<commit_message>
20250726 - Working Job Management
</commit_message>
<xml_diff>
--- a/github code.xlsx
+++ b/github code.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyApplication\ClaudeCode\Keith_Job_Management\Pilot\jobtracker-web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A154138-C4E5-4D2E-9D6C-6B721EB20662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDECA9D7-8B5D-4221-ACD5-1C7A445A83B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{881586A5-D68C-4AEB-AE74-D8630193A999}"/>
   </bookViews>
@@ -98,7 +98,7 @@
     <t>Let ChatGPT re-review with updated changes</t>
   </si>
   <si>
-    <t>git commit -m "20250721 - Working Chart"</t>
+    <t>git commit -m "20250726 - Working Job Management"</t>
   </si>
 </sst>
 </file>

</xml_diff>